<commit_message>
[FIX] Update AddAdherent + parsing GetPersonne
</commit_message>
<xml_diff>
--- a/Cognac-Behourd/Cognac-Behourd/Files/test.xlsx
+++ b/Cognac-Behourd/Cognac-Behourd/Files/test.xlsx
@@ -31,34 +31,62 @@
     <t>Paul</t>
   </si>
   <si>
-    <t>134kg</t>
-  </si>
-  <si>
     <t>BLANC</t>
   </si>
   <si>
     <t>Louis</t>
   </si>
   <si>
-    <t>47kg</t>
-  </si>
-  <si>
     <t>GIRAUD</t>
   </si>
   <si>
     <t>Jean-Michel</t>
   </si>
   <si>
-    <t>79kg</t>
-  </si>
-  <si>
     <t>PÂRIS</t>
   </si>
   <si>
     <t>Théophile</t>
   </si>
   <si>
-    <t>102kg</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Patate</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Chausette</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>300</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>2021</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -309,16 +337,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0" outlineLevelRow="8"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="9.38"/>
     <col customWidth="1" min="2" max="2" width="10.25"/>
     <col customWidth="1" min="3" max="3" width="9.38"/>
     <col customWidth="1" min="4" max="4" width="13.5"/>
-    <col customWidth="1" min="5" max="26" width="9.38"/>
+    <col customWidth="1" min="5" max="6" width="9.38"/>
+    <col customWidth="1" min="7" max="26" width="13.38"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" outlineLevel="8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -332,259 +361,277 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" outlineLevel="8">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
+      <c r="C2" s="1">
+        <v>134.0</v>
       </c>
       <c r="D2" s="1">
         <v>2006.0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" outlineLevel="8">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
+      <c r="C3" s="1">
+        <v>47.0</v>
       </c>
       <c r="D3" s="1">
         <v>2020.0</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" outlineLevel="8">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
+        <v>79.0</v>
       </c>
       <c r="D4" s="1">
         <v>1987.0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" outlineLevel="8">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="C5" s="1">
+        <v>102.0</v>
       </c>
       <c r="D5" s="1">
         <v>2003.0</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
-    <row r="97" ht="15.75" customHeight="1"/>
-    <row r="98" ht="15.75" customHeight="1"/>
-    <row r="99" ht="15.75" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1"/>
-    <row r="114" ht="15.75" customHeight="1"/>
-    <row r="115" ht="15.75" customHeight="1"/>
-    <row r="116" ht="15.75" customHeight="1"/>
-    <row r="117" ht="15.75" customHeight="1"/>
-    <row r="118" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="120" ht="15.75" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
-    <row r="126" ht="15.75" customHeight="1"/>
-    <row r="127" ht="15.75" customHeight="1"/>
-    <row r="128" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
-    <row r="134" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="136" ht="15.75" customHeight="1"/>
-    <row r="137" ht="15.75" customHeight="1"/>
-    <row r="138" ht="15.75" customHeight="1"/>
-    <row r="139" ht="15.75" customHeight="1"/>
-    <row r="140" ht="15.75" customHeight="1"/>
-    <row r="141" ht="15.75" customHeight="1"/>
-    <row r="142" ht="15.75" customHeight="1"/>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
-    <row r="147" ht="15.75" customHeight="1"/>
-    <row r="148" ht="15.75" customHeight="1"/>
-    <row r="149" ht="15.75" customHeight="1"/>
-    <row r="150" ht="15.75" customHeight="1"/>
-    <row r="151" ht="15.75" customHeight="1"/>
-    <row r="152" ht="15.75" customHeight="1"/>
-    <row r="153" ht="15.75" customHeight="1"/>
-    <row r="154" ht="15.75" customHeight="1"/>
-    <row r="155" ht="15.75" customHeight="1"/>
-    <row r="156" ht="15.75" customHeight="1"/>
-    <row r="157" ht="15.75" customHeight="1"/>
-    <row r="158" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
-    <row r="161" ht="15.75" customHeight="1"/>
-    <row r="162" ht="15.75" customHeight="1"/>
-    <row r="163" ht="15.75" customHeight="1"/>
-    <row r="164" ht="15.75" customHeight="1"/>
-    <row r="165" ht="15.75" customHeight="1"/>
-    <row r="166" ht="15.75" customHeight="1"/>
-    <row r="167" ht="15.75" customHeight="1"/>
-    <row r="168" ht="15.75" customHeight="1"/>
-    <row r="169" ht="15.75" customHeight="1"/>
-    <row r="170" ht="15.75" customHeight="1"/>
-    <row r="171" ht="15.75" customHeight="1"/>
-    <row r="172" ht="15.75" customHeight="1"/>
-    <row r="173" ht="15.75" customHeight="1"/>
-    <row r="174" ht="15.75" customHeight="1"/>
-    <row r="175" ht="15.75" customHeight="1"/>
-    <row r="176" ht="15.75" customHeight="1"/>
-    <row r="177" ht="15.75" customHeight="1"/>
-    <row r="178" ht="15.75" customHeight="1"/>
-    <row r="179" ht="15.75" customHeight="1"/>
-    <row r="180" ht="15.75" customHeight="1"/>
-    <row r="181" ht="15.75" customHeight="1"/>
-    <row r="182" ht="15.75" customHeight="1"/>
-    <row r="183" ht="15.75" customHeight="1"/>
-    <row r="184" ht="15.75" customHeight="1"/>
-    <row r="185" ht="15.75" customHeight="1"/>
-    <row r="186" ht="15.75" customHeight="1"/>
-    <row r="187" ht="15.75" customHeight="1"/>
-    <row r="188" ht="15.75" customHeight="1"/>
-    <row r="189" ht="15.75" customHeight="1"/>
-    <row r="190" ht="15.75" customHeight="1"/>
-    <row r="191" ht="15.75" customHeight="1"/>
-    <row r="192" ht="15.75" customHeight="1"/>
-    <row r="193" ht="15.75" customHeight="1"/>
-    <row r="194" ht="15.75" customHeight="1"/>
-    <row r="195" ht="15.75" customHeight="1"/>
-    <row r="196" ht="15.75" customHeight="1"/>
-    <row r="197" ht="15.75" customHeight="1"/>
-    <row r="198" ht="15.75" customHeight="1"/>
-    <row r="199" ht="15.75" customHeight="1"/>
-    <row r="200" ht="15.75" customHeight="1"/>
-    <row r="201" ht="15.75" customHeight="1"/>
-    <row r="202" ht="15.75" customHeight="1"/>
-    <row r="203" ht="15.75" customHeight="1"/>
-    <row r="204" ht="15.75" customHeight="1"/>
-    <row r="205" ht="15.75" customHeight="1"/>
-    <row r="206" ht="15.75" customHeight="1"/>
-    <row r="207" ht="15.75" customHeight="1"/>
-    <row r="208" ht="15.75" customHeight="1"/>
-    <row r="209" ht="15.75" customHeight="1"/>
-    <row r="210" ht="15.75" customHeight="1"/>
-    <row r="211" ht="15.75" customHeight="1"/>
-    <row r="212" ht="15.75" customHeight="1"/>
-    <row r="213" ht="15.75" customHeight="1"/>
-    <row r="214" ht="15.75" customHeight="1"/>
-    <row r="215" ht="15.75" customHeight="1"/>
-    <row r="216" ht="15.75" customHeight="1"/>
-    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="6" outlineLevel="6">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="18" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="19" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="20" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="21" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="22" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="23" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="24" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="25" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="26" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="27" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="28" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="29" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="30" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="31" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="32" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="33" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="34" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="35" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="36" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="37" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="38" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="39" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="40" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="41" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="42" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="43" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="44" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="45" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="46" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="47" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="48" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="49" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="50" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="51" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="52" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="53" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="54" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="55" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="56" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="57" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="58" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="59" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="60" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="61" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="62" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="63" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="64" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="65" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="66" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="67" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="68" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="69" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="70" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="71" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="72" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="73" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="74" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="75" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="76" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="77" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="78" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="79" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="80" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="81" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="82" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="83" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="84" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="85" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="86" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="87" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="88" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="89" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="90" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="91" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="92" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="93" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="94" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="95" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="96" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="97" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="98" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="99" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="100" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="101" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="102" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="103" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="104" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="105" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="106" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="107" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="108" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="109" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="110" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="111" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="112" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="113" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="114" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="115" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="116" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="117" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="118" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="119" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="120" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="121" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="122" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="123" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="124" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="125" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="126" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="127" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="128" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="129" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="130" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="131" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="132" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="133" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="134" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="135" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="136" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="137" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="138" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="139" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="140" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="141" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="142" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="143" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="144" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="145" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="146" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="147" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="148" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="149" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="150" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="151" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="152" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="153" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="154" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="155" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="156" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="157" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="158" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="159" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="160" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="161" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="162" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="163" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="164" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="165" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="166" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="167" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="168" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="169" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="170" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="171" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="172" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="173" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="174" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="175" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="176" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="177" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="178" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="179" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="180" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="181" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="182" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="183" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="184" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="185" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="186" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="187" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="188" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="189" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="190" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="191" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="192" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="193" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="194" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="195" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="196" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="197" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="198" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="199" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="200" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="201" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="202" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="203" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="204" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="205" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="206" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="207" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="208" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="209" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="210" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="211" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="212" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="213" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="214" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="215" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="216" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="217" ht="15.75" customHeight="1" outlineLevel="7"/>
     <row r="218" ht="15.75" customHeight="1"/>
     <row r="219" ht="15.75" customHeight="1"/>
     <row r="220" ht="15.75" customHeight="1"/>
@@ -1365,9 +1412,6 @@
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
[FIX/FEATURE] Refactor AddAdherent #23 + Ajouter les nouveau adhérent/visiteur dans la même collection de la liste de personne initié au début du programme #27
</commit_message>
<xml_diff>
--- a/Cognac-Behourd/Cognac-Behourd/Files/test.xlsx
+++ b/Cognac-Behourd/Cognac-Behourd/Files/test.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Nom</t>
   </si>
@@ -47,46 +47,6 @@
   </si>
   <si>
     <t>Théophile</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Patate</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Chausette</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>300</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>2021</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -344,7 +304,7 @@
     <col customWidth="1" min="3" max="3" width="9.38"/>
     <col customWidth="1" min="4" max="4" width="13.5"/>
     <col customWidth="1" min="5" max="6" width="9.38"/>
-    <col customWidth="1" min="7" max="26" width="13.38"/>
+    <col customWidth="1" min="7" max="26" width="15.5"/>
   </cols>
   <sheetData>
     <row r="1" outlineLevel="8">
@@ -417,20 +377,10 @@
         <v>2003.0</v>
       </c>
     </row>
-    <row r="6" outlineLevel="6">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
+    <row r="13" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="14" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="15" ht="15.75" customHeight="1" outlineLevel="8"/>
+    <row r="16" ht="15.75" customHeight="1" outlineLevel="8"/>
     <row r="17" ht="15.75" customHeight="1" outlineLevel="8"/>
     <row r="18" ht="15.75" customHeight="1" outlineLevel="8"/>
     <row r="19" ht="15.75" customHeight="1" outlineLevel="8"/>
@@ -628,10 +578,10 @@
     <row r="211" ht="15.75" customHeight="1" outlineLevel="8"/>
     <row r="212" ht="15.75" customHeight="1" outlineLevel="8"/>
     <row r="213" ht="15.75" customHeight="1" outlineLevel="8"/>
-    <row r="214" ht="15.75" customHeight="1" outlineLevel="8"/>
-    <row r="215" ht="15.75" customHeight="1" outlineLevel="8"/>
-    <row r="216" ht="15.75" customHeight="1" outlineLevel="8"/>
-    <row r="217" ht="15.75" customHeight="1" outlineLevel="7"/>
+    <row r="214" ht="15.75" customHeight="1" outlineLevel="7"/>
+    <row r="215" ht="15.75" customHeight="1" outlineLevel="7"/>
+    <row r="216" ht="15.75" customHeight="1" outlineLevel="7"/>
+    <row r="217" ht="15.75" customHeight="1" outlineLevel="6"/>
     <row r="218" ht="15.75" customHeight="1"/>
     <row r="219" ht="15.75" customHeight="1"/>
     <row r="220" ht="15.75" customHeight="1"/>

</xml_diff>